<commit_message>
carpetas csv's y esquema BBDD actualizado
</commit_message>
<xml_diff>
--- a/BBDD.xlsx
+++ b/BBDD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Adalab\modulo-2\modulo-2-proyecto\proyecto-da-promo-Farzana-modulo2-team5-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarag\Desktop\Adalab\modulo-2\m2-proyecto\proyecto-da-promo-Farzana-modulo2-team5-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AFCFDF4-B1AB-475E-9D14-DFE08C917BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1086D3F-6A32-4E90-A10F-7E76C7095F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="-15" windowWidth="21600" windowHeight="11295" xr2:uid="{CC97AF95-2AAD-4CF3-9470-FF4676C0924D}"/>
+    <workbookView xWindow="-105" yWindow="1875" windowWidth="21600" windowHeight="11295" xr2:uid="{CC97AF95-2AAD-4CF3-9470-FF4676C0924D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>peliculas</t>
   </si>
@@ -49,9 +49,6 @@
     <t>mes</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>puntos</t>
   </si>
   <si>
@@ -131,6 +128,36 @@
   </si>
   <si>
     <t>guionista</t>
+  </si>
+  <si>
+    <t>actor</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>id peli</t>
+  </si>
+  <si>
+    <t>actors</t>
+  </si>
+  <si>
+    <t>actores eli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actores </t>
+  </si>
+  <si>
+    <t>peliculas_api_1998</t>
+  </si>
+  <si>
+    <t>peliculas_raw</t>
+  </si>
+  <si>
+    <t>datos_imdb</t>
+  </si>
+  <si>
+    <t>datos_imdb:_1998</t>
   </si>
 </sst>
 </file>
@@ -174,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -197,19 +224,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -222,9 +236,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA03CF6-9571-4C5B-ACC8-C7C81BF00E31}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,29 +570,29 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>2</v>
@@ -585,97 +601,147 @@
         <v>3</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="K13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -697,23 +763,23 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>